<commit_message>
Se modifica archivo gitignore
</commit_message>
<xml_diff>
--- a/companies2.xlsx
+++ b/companies2.xlsx
@@ -38,7 +38,10 @@
     <t xml:space="preserve">Telefono</t>
   </si>
   <si>
-    <t xml:space="preserve">Categoria</t>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Category</t>
   </si>
   <si>
     <t xml:space="preserve">Yo</t>
@@ -51,6 +54,15 @@
   </si>
   <si>
     <t xml:space="preserve">45454</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alimentaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMPERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45454sdsdsd</t>
   </si>
 </sst>
 </file>
@@ -391,39 +403,108 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>20</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>202</v>
       </c>
       <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="C4">
+        <v>202</v>
+      </c>
+      <c r="D4" t="s">
         <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>202</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <v>202</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se modifica el archivo excel
</commit_message>
<xml_diff>
--- a/companies2.xlsx
+++ b/companies2.xlsx
@@ -44,7 +44,7 @@
     <t xml:space="preserve">Category</t>
   </si>
   <si>
-    <t xml:space="preserve">Yo</t>
+    <t xml:space="preserve">CAMPERO</t>
   </si>
   <si>
     <t xml:space="preserve">Alto</t>
@@ -53,16 +53,16 @@
     <t xml:space="preserve">2255789</t>
   </si>
   <si>
-    <t xml:space="preserve">45454</t>
+    <t xml:space="preserve">45454sdsdsd</t>
   </si>
   <si>
     <t xml:space="preserve">Alimentaria</t>
   </si>
   <si>
-    <t xml:space="preserve">CAMPERO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45454sdsdsd</t>
+    <t xml:space="preserve">CAMPERO2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMPERO23</t>
   </si>
 </sst>
 </file>
@@ -386,6 +386,9 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="11" max="11" width="30" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -415,7 +418,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>20</v>
+        <v>202</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -429,7 +432,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
@@ -449,7 +452,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
@@ -464,46 +467,6 @@
         <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>202</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>202</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Se modifica el archivo excel de ejemplo
</commit_message>
<xml_diff>
--- a/companies2.xlsx
+++ b/companies2.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djohnson\Code\xlsx-populate\lib\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\IN6AMDilan\COPEREX\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04333DE1-1289-40B8-AAAF-417F051882E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="23070" windowHeight="10320" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,53 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <si>
-    <t xml:space="preserve">Nombre de la Empresa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nivel de impacto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Años de trayectoria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Telefono</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Email</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Category</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2255789</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45454</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alimentaria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAMPERO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45454sdsdsd</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts/>
-  <fonts x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,7 +39,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills>
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -87,7 +47,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -99,7 +59,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs>
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -380,142 +340,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="20" customWidth="1"/>
+    <col min="2" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="30" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
   </cols>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>202</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>202</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>202</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6">
-        <v>202</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>